<commit_message>
add csv map for login member institution
</commit_message>
<xml_diff>
--- a/UserManagement/wwwroot/InputExcel/eSanjeevaniAB Demo.xlsx
+++ b/UserManagement/wwwroot/InputExcel/eSanjeevaniAB Demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <r>
       <rPr>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">City</t>
   </si>
   <si>
-    <t xml:space="preserve">Address  </t>
+    <t xml:space="preserve">Address</t>
   </si>
   <si>
     <t xml:space="preserve">PIN</t>
@@ -115,8 +115,7 @@
 /Designation</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of Birth 
-DD-MM-YYYY</t>
+    <t xml:space="preserve">Date of Birth DD-MM-YYYY</t>
   </si>
   <si>
     <t xml:space="preserve">User State</t>
@@ -173,6 +172,9 @@
     <t xml:space="preserve">ABU ROAD</t>
   </si>
   <si>
+    <t xml:space="preserve">rajesh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kumar</t>
   </si>
   <si>
@@ -182,13 +184,13 @@
     <t xml:space="preserve">GNM</t>
   </si>
   <si>
-    <t xml:space="preserve">rajeshcdactest@cdac.com</t>
+    <t xml:space="preserve">rajeshcdacdemo@cdac.com</t>
   </si>
   <si>
     <t xml:space="preserve">CHO</t>
   </si>
   <si>
-    <t xml:space="preserve">10.10.1981</t>
+    <t xml:space="preserve">10-10-1981</t>
   </si>
   <si>
     <t xml:space="preserve">Dr</t>
@@ -215,10 +217,16 @@
     <t xml:space="preserve">ABOHAR</t>
   </si>
   <si>
+    <t xml:space="preserve">ABHOR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Faizal</t>
   </si>
   <si>
-    <t xml:space="preserve">faizal1@gmail.com</t>
+    <t xml:space="preserve">aaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faizal1demo@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">HWC Majra</t>
@@ -429,16 +437,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -524,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,7 +557,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="55.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.75"/>
@@ -603,7 +611,7 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -738,33 +746,35 @@
       <c r="K3" s="9" t="n">
         <v>87299</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="13" t="n">
-        <v>8728822888</v>
+      <c r="M3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="14" t="n">
+        <v>9728822877</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="13" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="14" t="n">
         <v>19</v>
       </c>
       <c r="R3" s="3" t="n">
         <v>23929999</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>44</v>
+      <c r="S3" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>38</v>
@@ -782,10 +792,10 @@
         <v>989999</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC3" s="15" t="n">
         <v>0.395833333333333</v>
@@ -798,15 +808,15 @@
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>23990230</v>
@@ -818,71 +828,73 @@
         <v>12345678</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K4" s="9" t="n">
         <v>122233</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13" t="n">
-        <v>9338057314</v>
+        <v>57</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="14" t="n">
+        <v>8338057323</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="13" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="14" t="n">
         <v>19</v>
       </c>
       <c r="R4" s="3" t="n">
         <v>23989839</v>
       </c>
-      <c r="S4" s="14" t="s">
-        <v>56</v>
+      <c r="S4" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z4" s="3" t="n">
         <v>120900</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC4" s="15" t="n">
         <v>0.395833333333333</v>
@@ -895,9 +907,10 @@
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
change sequence and fix the mapping for member slot
</commit_message>
<xml_diff>
--- a/UserManagement/wwwroot/InputExcel/eSanjeevaniAB Demo.xlsx
+++ b/UserManagement/wwwroot/InputExcel/eSanjeevaniAB Demo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
   <si>
     <r>
       <rPr>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">GNM</t>
   </si>
   <si>
-    <t xml:space="preserve">rajeshcdacdemo@cdac.com</t>
+    <t xml:space="preserve">rajesh121@cdac.com</t>
   </si>
   <si>
     <t xml:space="preserve">CHO</t>
@@ -226,10 +226,79 @@
     <t xml:space="preserve">aaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">faizal1demo@gmail.com</t>
+    <t xml:space="preserve">faizal111@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-06-1982</t>
   </si>
   <si>
     <t xml:space="preserve">HWC Majra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB Dipali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dipali@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAHARASHTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pune Dipali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dipali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaikwad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEMALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dipali@cdac.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-09-1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPHC Elina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elina@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KARNATAKA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENGALURU URBAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENGALURU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENGALURU Elina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nagtilak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elina@cdac.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-06-1984</t>
   </si>
 </sst>
 </file>
@@ -240,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-C09]H:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -332,6 +401,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -388,7 +463,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -451,6 +526,14 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -532,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA6" activeCellId="0" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -557,7 +640,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="55.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.75"/>
@@ -753,7 +836,7 @@
         <v>42</v>
       </c>
       <c r="N3" s="14" t="n">
-        <v>9728822877</v>
+        <v>9228822877</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>43</v>
@@ -852,7 +935,7 @@
         <v>58</v>
       </c>
       <c r="N4" s="14" t="n">
-        <v>8338057323</v>
+        <v>8438057323</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>43</v>
@@ -873,7 +956,7 @@
         <v>46</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="V4" s="11" t="s">
         <v>53</v>
@@ -907,10 +990,207 @@
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>29382939</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>34092030</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="9" t="n">
+        <v>87299</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="14" t="n">
+        <v>8598696854</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>23929999</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z5" s="3" t="n">
+        <v>989999</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="15" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="AD5" s="15" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>23990230</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="9" t="n">
+        <v>122233</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="14" t="n">
+        <v>9952418751</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>23989839</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="X6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z6" s="3" t="n">
+        <v>120900</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC6" s="15" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="AD6" s="15" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="AE6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1896,6 +2176,10 @@
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="L1:Z1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" display="Elina@gmail.com"/>
+    <hyperlink ref="S6" r:id="rId2" display="elina@cdac.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="95" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>